<commit_message>
update data for case study
</commit_message>
<xml_diff>
--- a/casestudy/countries-and-timezones-60/results.xlsx
+++ b/casestudy/countries-and-timezones-60/results.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10209"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10315"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/franktip/git/mutation-testing-data/casestudy/countries-and-timezones-60/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB58AA64-EFD0-A54D-AAFF-B942AF7167BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B00291B-3A2A-F54A-8836-521932598C6F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7360" yWindow="7400" windowWidth="27240" windowHeight="16440" activeTab="3" xr2:uid="{BA8F4140-1AF3-1848-B3E0-7ADBCED5078A}"/>
+    <workbookView xWindow="7360" yWindow="7400" windowWidth="27240" windowHeight="16440" activeTab="4" xr2:uid="{BA8F4140-1AF3-1848-B3E0-7ADBCED5078A}"/>
   </bookViews>
   <sheets>
-    <sheet name="run1" sheetId="1" r:id="rId1"/>
+    <sheet name="run1" sheetId="4" r:id="rId1"/>
     <sheet name="run 2" sheetId="2" r:id="rId2"/>
     <sheet name="run3" sheetId="3" r:id="rId3"/>
-    <sheet name="run4" sheetId="4" r:id="rId4"/>
+    <sheet name="run4" sheetId="1" r:id="rId4"/>
     <sheet name="run5" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="181029"/>
@@ -682,7 +682,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -696,7 +696,15 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1030,19 +1038,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{45260694-0BBD-5143-B71E-4CB7D6F62B75}">
-  <dimension ref="A1:H12"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2D8478CE-4E42-ED49-86FC-D0F1E49FB7E9}">
+  <dimension ref="A1:H11"/>
   <sheetViews>
     <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10:C10"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="38.6640625" customWidth="1"/>
-    <col min="2" max="2" width="32.83203125" customWidth="1"/>
-    <col min="3" max="3" width="40" customWidth="1"/>
-    <col min="8" max="8" width="36.83203125" customWidth="1"/>
+    <col min="1" max="1" width="35.83203125" customWidth="1"/>
+    <col min="2" max="2" width="28.33203125" customWidth="1"/>
+    <col min="3" max="3" width="32.83203125" customWidth="1"/>
+    <col min="8" max="8" width="43.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.2">
@@ -1063,14 +1071,14 @@
         <v>29</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="289" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:8" ht="323" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="6" t="s">
         <v>14</v>
       </c>
       <c r="H2" s="2" t="s">
@@ -1079,111 +1087,100 @@
     </row>
     <row r="3" spans="1:8" ht="204" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>1</v>
+        <v>40</v>
       </c>
       <c r="B3" t="s">
-        <v>12</v>
-      </c>
-      <c r="C3" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" ht="289" x14ac:dyDescent="0.2">
+        <v>39</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="221" x14ac:dyDescent="0.2">
+      <c r="A5" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5" s="6" t="s">
         <v>14</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" ht="388" x14ac:dyDescent="0.2">
-      <c r="A5" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="C5" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="204" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="C6" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" ht="289" x14ac:dyDescent="0.2">
+        <v>41</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="204" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="C7" t="s">
+        <v>21</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="323" x14ac:dyDescent="0.2">
+      <c r="A8" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C8" s="6" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="204" x14ac:dyDescent="0.2">
-      <c r="A8" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="C8" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" ht="289" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:8" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="C9" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" ht="388" x14ac:dyDescent="0.2">
+        <v>8</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="C9" s="7" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="204" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
-        <v>8</v>
+        <v>38</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="C10" t="s">
-        <v>18</v>
+        <v>39</v>
+      </c>
+      <c r="C10" s="6" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="11" spans="1:8" ht="238" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
-        <v>9</v>
+        <v>43</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="C11" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" ht="388" x14ac:dyDescent="0.2">
-      <c r="A12" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="C12" t="s">
+        <v>46</v>
+      </c>
+      <c r="C11" s="6" t="s">
         <v>18</v>
       </c>
     </row>
@@ -1196,8 +1193,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{62C430C8-EF7C-864F-9C13-90FBBD429C35}">
   <dimension ref="A1:H11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1234,7 +1231,7 @@
       <c r="B2" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="6" t="s">
         <v>14</v>
       </c>
       <c r="H2" s="2" t="s">
@@ -1248,7 +1245,7 @@
       <c r="B3" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="6" t="s">
         <v>14</v>
       </c>
     </row>
@@ -1259,7 +1256,7 @@
       <c r="B4" t="s">
         <v>12</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="6" t="s">
         <v>12</v>
       </c>
     </row>
@@ -1270,7 +1267,7 @@
       <c r="B5" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" s="6" t="s">
         <v>18</v>
       </c>
     </row>
@@ -1281,7 +1278,7 @@
       <c r="B6" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" s="6" t="s">
         <v>14</v>
       </c>
     </row>
@@ -1292,7 +1289,7 @@
       <c r="B7" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C7" s="6" t="s">
         <v>18</v>
       </c>
     </row>
@@ -1303,7 +1300,7 @@
       <c r="B8" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C8" s="6" t="s">
         <v>18</v>
       </c>
     </row>
@@ -1314,7 +1311,7 @@
       <c r="B9" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C9" s="6" t="s">
         <v>18</v>
       </c>
     </row>
@@ -1325,7 +1322,7 @@
       <c r="B10" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C10" s="6" t="s">
         <v>18</v>
       </c>
     </row>
@@ -1336,7 +1333,7 @@
       <c r="B11" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C11" s="6" t="s">
         <v>18</v>
       </c>
     </row>
@@ -1349,7 +1346,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{611F4CE5-1A94-D544-828F-3756B1B1292E}">
   <dimension ref="A1:H11"/>
   <sheetViews>
-    <sheetView topLeftCell="A11" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
@@ -1386,21 +1383,21 @@
       <c r="B2" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="6" t="s">
         <v>14</v>
       </c>
       <c r="H2" s="2" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="255" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:8" ht="204" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>36</v>
       </c>
       <c r="B3" t="s">
         <v>39</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="6" t="s">
         <v>39</v>
       </c>
     </row>
@@ -1411,7 +1408,7 @@
       <c r="B4" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="6" t="s">
         <v>18</v>
       </c>
     </row>
@@ -1422,7 +1419,7 @@
       <c r="B5" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" s="6" t="s">
         <v>14</v>
       </c>
     </row>
@@ -1433,7 +1430,7 @@
       <c r="B6" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" s="6" t="s">
         <v>18</v>
       </c>
     </row>
@@ -1444,7 +1441,7 @@
       <c r="B7" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C7" s="6" t="s">
         <v>18</v>
       </c>
     </row>
@@ -1455,7 +1452,7 @@
       <c r="B8" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C8" s="6" t="s">
         <v>18</v>
       </c>
     </row>
@@ -1466,7 +1463,7 @@
       <c r="B9" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C9" s="6" t="s">
         <v>18</v>
       </c>
     </row>
@@ -1477,7 +1474,7 @@
       <c r="B10" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C10" s="6" t="s">
         <v>39</v>
       </c>
     </row>
@@ -1488,7 +1485,7 @@
       <c r="B11" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C11" s="6" t="s">
         <v>18</v>
       </c>
     </row>
@@ -1498,19 +1495,19 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2D8478CE-4E42-ED49-86FC-D0F1E49FB7E9}">
-  <dimension ref="A1:H11"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{45260694-0BBD-5143-B71E-4CB7D6F62B75}">
+  <dimension ref="A1:H12"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10:C10"/>
+    <sheetView topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="35.83203125" customWidth="1"/>
-    <col min="2" max="2" width="28.33203125" customWidth="1"/>
-    <col min="3" max="3" width="32.83203125" customWidth="1"/>
-    <col min="8" max="8" width="43.6640625" customWidth="1"/>
+    <col min="1" max="1" width="38.6640625" customWidth="1"/>
+    <col min="2" max="2" width="32.83203125" customWidth="1"/>
+    <col min="3" max="3" width="40" customWidth="1"/>
+    <col min="8" max="8" width="36.83203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.2">
@@ -1531,14 +1528,14 @@
         <v>29</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="323" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:8" ht="289" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="6" t="s">
         <v>14</v>
       </c>
       <c r="H2" s="2" t="s">
@@ -1547,100 +1544,111 @@
     </row>
     <row r="3" spans="1:8" ht="204" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>40</v>
+        <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>39</v>
-      </c>
-      <c r="C3" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" ht="409.6" x14ac:dyDescent="0.2">
+        <v>12</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="289" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="388" x14ac:dyDescent="0.2">
+      <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B5" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C4" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" ht="221" x14ac:dyDescent="0.2">
-      <c r="A5" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C5" t="s">
-        <v>14</v>
+      <c r="C5" s="6" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="204" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
-        <v>41</v>
+        <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" ht="204" x14ac:dyDescent="0.2">
+        <v>19</v>
+      </c>
+      <c r="C6" s="6" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="289" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="204" x14ac:dyDescent="0.2">
+      <c r="A8" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="B8" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="C7" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" ht="323" x14ac:dyDescent="0.2">
-      <c r="A8" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="C8" t="s">
+      <c r="C8" s="6" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="289" x14ac:dyDescent="0.2">
+      <c r="A9" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C9" s="6" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="9" spans="1:8" ht="409.6" x14ac:dyDescent="0.2">
-      <c r="A9" s="1" t="s">
+    <row r="10" spans="1:8" ht="388" x14ac:dyDescent="0.2">
+      <c r="A10" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B9" s="4" t="s">
+      <c r="B10" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="C9" s="5" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" ht="204" x14ac:dyDescent="0.2">
-      <c r="A10" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="C10" t="s">
-        <v>39</v>
+      <c r="C10" s="6" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="11" spans="1:8" ht="238" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
-        <v>43</v>
+        <v>9</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="C11" t="s">
+        <v>24</v>
+      </c>
+      <c r="C11" s="6" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" ht="388" x14ac:dyDescent="0.2">
+      <c r="A12" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C12" s="6" t="s">
         <v>18</v>
       </c>
     </row>
@@ -1653,8 +1661,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4BAD8DAD-99CB-094E-8B83-51C6C4237597}">
   <dimension ref="A1:H10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1690,7 +1698,7 @@
       <c r="B2" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="6" t="s">
         <v>14</v>
       </c>
       <c r="H2" s="2" t="s">
@@ -1704,7 +1712,7 @@
       <c r="B3" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="6" t="s">
         <v>52</v>
       </c>
     </row>
@@ -1715,7 +1723,7 @@
       <c r="B4" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="6" t="s">
         <v>18</v>
       </c>
     </row>
@@ -1726,7 +1734,7 @@
       <c r="B5" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" s="6" t="s">
         <v>14</v>
       </c>
     </row>
@@ -1737,7 +1745,7 @@
       <c r="B6" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" s="6" t="s">
         <v>18</v>
       </c>
     </row>
@@ -1748,7 +1756,7 @@
       <c r="B7" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C7" s="6" t="s">
         <v>18</v>
       </c>
     </row>
@@ -1759,7 +1767,7 @@
       <c r="B8" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C8" s="6" t="s">
         <v>14</v>
       </c>
     </row>
@@ -1770,7 +1778,7 @@
       <c r="B9" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C9" s="6" t="s">
         <v>18</v>
       </c>
     </row>
@@ -1781,7 +1789,7 @@
       <c r="B10" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C10" s="6" t="s">
         <v>39</v>
       </c>
     </row>

</xml_diff>